<commit_message>
jobticket template missing data
</commit_message>
<xml_diff>
--- a/app/webroot/img/jobticket.xlsx
+++ b/app/webroot/img/jobticket.xlsx
@@ -120,7 +120,7 @@
       <patternFill patternType="none"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -382,11 +382,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -425,44 +462,25 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -475,24 +493,47 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -794,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B12"/>
+      <selection activeCell="A14" sqref="A14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,52 +853,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="27"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="21" t="s">
         <v>4</v>
       </c>
@@ -876,8 +917,8 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -889,8 +930,8 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
@@ -902,8 +943,8 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
@@ -915,79 +956,79 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="42"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="43"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="44"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="49"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39" t="s">
+      <c r="B14" s="30"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="B15" s="33"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -1052,7 +1093,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1061,24 +1102,34 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="15">
-    <mergeCell ref="A13:C13"/>
+  <mergeCells count="16">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>